<commit_message>
start in plotting benchmark
</commit_message>
<xml_diff>
--- a/Task 4/Code/Planes_Data/B747_FC5.xlsx
+++ b/Task 4/Code/Planes_Data/B747_FC5.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\forth year\second term\control\Task_3\Task_4\Task_4_final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\4th year\Second term\Design of Control Systems for Aeronautical and Space Vehicles _ AER4420\Project\Autopilot-project\Task 4\Code\Planes_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD9B795-703C-4B40-928D-272A6F3F10F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -449,7 +455,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -652,7 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -663,9 +669,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -691,13 +696,13 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1199,11 +1204,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,11 +1229,11 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1240,10 +1245,10 @@
       <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>20000</v>
       </c>
     </row>
@@ -1252,15 +1257,15 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>300</v>
+        <v>1200</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>0.5</v>
       </c>
     </row>
@@ -1274,10 +1279,10 @@
       <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>518</v>
       </c>
     </row>
@@ -1292,10 +1297,10 @@
       <c r="C5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>307</v>
       </c>
     </row>
@@ -1310,10 +1315,10 @@
       <c r="C6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>228</v>
       </c>
     </row>
@@ -1328,10 +1333,10 @@
       <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>636636</v>
       </c>
     </row>
@@ -1343,8 +1348,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1356,10 +1360,10 @@
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>18200000</v>
       </c>
     </row>
@@ -1373,8 +1377,8 @@
       <c r="C10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="11">
+      <c r="D10" s="25"/>
+      <c r="E10" s="10">
         <v>33100000</v>
       </c>
     </row>
@@ -1388,8 +1392,8 @@
       <c r="C11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="11">
+      <c r="D11" s="25"/>
+      <c r="E11" s="10">
         <v>49700000</v>
       </c>
     </row>
@@ -1404,8 +1408,8 @@
       <c r="C12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="11">
+      <c r="D12" s="25"/>
+      <c r="E12" s="10">
         <v>970056</v>
       </c>
     </row>
@@ -1420,10 +1424,10 @@
       <c r="C13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>-1.76</v>
       </c>
     </row>
@@ -1438,10 +1442,10 @@
       <c r="C14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>170</v>
       </c>
     </row>
@@ -1456,13 +1460,13 @@
       <c r="C15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>181</v>
       </c>
-      <c r="I15" s="19"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1475,15 +1479,15 @@
       <c r="C16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>6.8</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>125</v>
       </c>
       <c r="B17" s="6">
@@ -1493,15 +1497,15 @@
       <c r="C17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="6">
@@ -1509,19 +1513,18 @@
         <v>0.5</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>86</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>84</v>
       </c>
       <c r="B19" s="6">
@@ -1529,17 +1532,16 @@
         <v>0.11868238913561441</v>
       </c>
       <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>-10</v>
       </c>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="16" t="s">
         <v>82</v>
       </c>
       <c r="B20" s="6">
@@ -1549,19 +1551,19 @@
       <c r="C20" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="10">
         <v>2.5</v>
       </c>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>83</v>
       </c>
       <c r="B21" s="1">
@@ -1571,16 +1573,16 @@
       <c r="C21" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="10">
         <v>2.5</v>
       </c>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
@@ -1593,16 +1595,16 @@
       <c r="C22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="10">
         <v>10</v>
       </c>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
@@ -1612,15 +1614,15 @@
         <f t="shared" si="0"/>
         <v>-6.7900000000000002E-2</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
@@ -1633,16 +1635,16 @@
       <c r="C24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="10">
         <v>20000</v>
       </c>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
@@ -1655,10 +1657,10 @@
       <c r="C25" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="10">
         <v>0.5</v>
       </c>
     </row>
@@ -1673,10 +1675,10 @@
       <c r="C26" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="10">
         <v>-2.47E-3</v>
       </c>
     </row>
@@ -1691,10 +1693,10 @@
       <c r="C27" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="10">
         <v>-6.7900000000000002E-2</v>
       </c>
     </row>
@@ -1709,10 +1711,10 @@
       <c r="C28" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" t="s">
         <v>76</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="10">
         <v>2.4699999999999999E-4</v>
       </c>
     </row>
@@ -1727,10 +1729,10 @@
       <c r="C29" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="10">
         <v>7.8200000000000006E-2</v>
       </c>
     </row>
@@ -1745,10 +1747,10 @@
       <c r="C30" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="10">
         <v>-0.433</v>
       </c>
     </row>
@@ -1763,10 +1765,10 @@
       <c r="C31" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" t="s">
         <v>76</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="10">
         <v>-1.6999999999999999E-3</v>
       </c>
     </row>
@@ -1781,10 +1783,10 @@
       <c r="C32" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="10">
         <v>1.5699999999999999E-2</v>
       </c>
     </row>
@@ -1799,10 +1801,10 @@
       <c r="C33" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="10">
         <v>-6.39</v>
       </c>
     </row>
@@ -1817,10 +1819,10 @@
       <c r="C34" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="10">
         <v>-1.25E-4</v>
       </c>
     </row>
@@ -1835,10 +1837,10 @@
       <c r="C35" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="10">
         <v>-0.42099999999999999</v>
       </c>
     </row>
@@ -1853,10 +1855,10 @@
       <c r="C36" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E36" s="10">
         <v>2.02</v>
       </c>
     </row>
@@ -1871,10 +1873,10 @@
       <c r="C37" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" t="s">
         <v>78</v>
       </c>
-      <c r="E37" s="11">
+      <c r="E37" s="10">
         <v>-16.899999999999999</v>
       </c>
     </row>
@@ -1889,10 +1891,10 @@
       <c r="C38" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" t="s">
         <v>79</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E38" s="10">
         <v>-1.0900000000000001</v>
       </c>
     </row>
@@ -1907,8 +1909,7 @@
       <c r="C39" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11">
+      <c r="E39" s="10">
         <v>5.0500000000000001E-5</v>
       </c>
     </row>
@@ -1923,8 +1924,7 @@
       <c r="C40" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="11">
+      <c r="E40" s="10">
         <v>-2.2000000000000001E-6</v>
       </c>
     </row>
@@ -1939,8 +1939,7 @@
       <c r="C41" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11">
+      <c r="E41" s="10">
         <v>3.0199999999999998E-7</v>
       </c>
     </row>
@@ -1952,11 +1951,11 @@
         <f t="shared" si="1"/>
         <v>-0.65200000000000002</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="21"/>
-      <c r="E42" s="22"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="21"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
@@ -1969,10 +1968,10 @@
       <c r="C43" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="11">
+      <c r="E43" s="10">
         <v>20000</v>
       </c>
     </row>
@@ -1987,10 +1986,10 @@
       <c r="C44" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E44" s="11">
+      <c r="E44" s="10">
         <v>0.5</v>
       </c>
     </row>
@@ -2005,10 +2004,10 @@
       <c r="C45" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" t="s">
         <v>75</v>
       </c>
-      <c r="E45" s="11">
+      <c r="E45" s="10">
         <v>-8.2199999999999995E-2</v>
       </c>
     </row>
@@ -2023,10 +2022,10 @@
       <c r="C46" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" t="s">
         <v>80</v>
       </c>
-      <c r="E46" s="11">
+      <c r="E46" s="10">
         <v>-42.6</v>
       </c>
     </row>
@@ -2041,10 +2040,10 @@
       <c r="C47" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="11">
+      <c r="E47" s="10">
         <v>-2.0499999999999998</v>
       </c>
     </row>
@@ -2059,10 +2058,10 @@
       <c r="C48" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" t="s">
         <v>81</v>
       </c>
-      <c r="E48" s="11">
+      <c r="E48" s="10">
         <v>0.41899999999999998</v>
       </c>
     </row>
@@ -2077,10 +2076,10 @@
       <c r="C49" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" t="s">
         <v>75</v>
       </c>
-      <c r="E49" s="11">
+      <c r="E49" s="10">
         <v>-0.65200000000000002</v>
       </c>
     </row>
@@ -2095,10 +2094,10 @@
       <c r="C50" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D50" t="s">
         <v>75</v>
       </c>
-      <c r="E50" s="11">
+      <c r="E50" s="10">
         <v>-7.0099999999999996E-2</v>
       </c>
     </row>
@@ -2113,15 +2112,15 @@
       <c r="C51" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" t="s">
         <v>75</v>
       </c>
-      <c r="E51" s="11">
+      <c r="E51" s="10">
         <v>0.376</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
+      <c r="A52" s="17" t="s">
         <v>118</v>
       </c>
       <c r="B52" s="1">
@@ -2131,15 +2130,15 @@
       <c r="C52" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D52" t="s">
         <v>75</v>
       </c>
-      <c r="E52" s="11">
+      <c r="E52" s="10">
         <v>-0.14000000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="17" t="s">
         <v>119</v>
       </c>
       <c r="B53" s="1">
@@ -2148,15 +2147,15 @@
       <c r="C53" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" t="s">
         <v>75</v>
       </c>
-      <c r="E53" s="11">
+      <c r="E53" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="17" t="s">
         <v>120</v>
       </c>
       <c r="B54" s="6">
@@ -2166,15 +2165,15 @@
       <c r="C54" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" t="s">
         <v>77</v>
       </c>
-      <c r="E54" s="11">
+      <c r="E54" s="10">
         <v>0.128</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="17" t="s">
         <v>121</v>
       </c>
       <c r="B55" s="6">
@@ -2184,15 +2183,15 @@
       <c r="C55" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" t="s">
         <v>77</v>
       </c>
-      <c r="E55" s="11">
+      <c r="E55" s="10">
         <v>1.77E-2</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="17" t="s">
         <v>122</v>
       </c>
       <c r="B56" s="6">
@@ -2202,15 +2201,15 @@
       <c r="C56" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" t="s">
         <v>75</v>
       </c>
-      <c r="E56" s="11">
+      <c r="E56" s="10">
         <v>1.3100000000000001E-2</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
+      <c r="A57" s="17" t="s">
         <v>123</v>
       </c>
       <c r="B57" s="6">
@@ -2220,10 +2219,10 @@
       <c r="C57" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D57" t="s">
         <v>77</v>
       </c>
-      <c r="E57" s="11">
+      <c r="E57" s="10">
         <v>0.14799999999999999</v>
       </c>
     </row>
@@ -2234,13 +2233,13 @@
       <c r="B58" s="1">
         <v>0</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="E58" s="16">
+      <c r="E58" s="15">
         <v>-0.38100000000000001</v>
       </c>
     </row>
@@ -2267,63 +2266,63 @@
       <c r="B61" s="1">
         <v>0</v>
       </c>
-      <c r="C61" s="24" t="s">
+      <c r="C61" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23"/>
     </row>
     <row r="64" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>

</xml_diff>